<commit_message>
add feature modal option student
</commit_message>
<xml_diff>
--- a/web/uploads/data-student (1).xlsx
+++ b/web/uploads/data-student (1).xlsx
@@ -94,7 +94,7 @@
     <t>0338188506</t>
   </si>
   <si>
-    <t>{"type":"Buffer","data":[0]}</t>
+    <t>{"type":"Buffer","data":[1]}</t>
   </si>
 </sst>
 </file>
@@ -417,7 +417,7 @@
     </row>
     <row r="2">
       <c r="A2" s="2">
-        <v>1.9524792E7</v>
+        <v>1.9524795E7</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>17</v>
@@ -458,7 +458,7 @@
       <c r="N2" s="1">
         <v>2.4610447E7</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="O2" s="2" t="s">
         <v>27</v>
       </c>
       <c r="P2" s="1">

</xml_diff>